<commit_message>
added horizontal flip to train transforms
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="54">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -163,10 +163,25 @@
     <t xml:space="preserve">resnext50_32x4d_12</t>
   </si>
   <si>
+    <t xml:space="preserve">Хуже, чем 10й запуск с Radam lr=0.001</t>
+  </si>
+  <si>
     <t xml:space="preserve">resnext50_32x4d_00_fold0</t>
   </si>
   <si>
     <t xml:space="preserve">resnext50_32x4d_00_fold1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resnext50_32x4d_00_fold2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resnext50_32x4d_00_fold3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resnext50_32x4d_00_fold4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resnext50_32x4d_00_folds</t>
   </si>
 </sst>
 </file>
@@ -342,10 +357,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="topLeft" activeCell="L22" activeCellId="0" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -946,12 +961,18 @@
       <c r="F15" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="H15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="I15" s="2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="K15" s="2" t="n">
         <v>1</v>
       </c>
@@ -981,16 +1002,25 @@
       <c r="H16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="I16" s="0" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="K16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L16" s="2" t="n">
         <v>0.485</v>
       </c>
+      <c r="M16" s="0" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>20</v>
@@ -1007,12 +1037,18 @@
       <c r="F17" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="0" t="n">
+        <v>44</v>
+      </c>
       <c r="H17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="I17" s="2" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>9.43</v>
+      </c>
       <c r="K17" s="2" t="n">
         <v>1</v>
       </c>
@@ -1022,7 +1058,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
@@ -1039,16 +1075,140 @@
       <c r="F18" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="n">
+        <v>32</v>
+      </c>
       <c r="H18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="I18" s="2" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>9.19</v>
+      </c>
       <c r="K18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L18" s="2" t="n">
+        <v>0.485</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>512</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>0.485</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>512</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>0.485</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>512</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>0.485</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2" t="n">
         <v>0.485</v>
       </c>
     </row>

</xml_diff>